<commit_message>
updated the time calculation in run_multiple_scenarios_domain_reduction.py
</commit_message>
<xml_diff>
--- a/data/Toy instance/Scenario Map Toy 2.xlsx
+++ b/data/Toy instance/Scenario Map Toy 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/j_callesalazar_deakin_edu_au/Documents/calle test/Disun Applications/Gurobi Applications/data/Toy instance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="8_{FB5113DB-7A77-4994-B7F3-4AEA239B3CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66B50C71-9147-4D3B-8D23-C244331F546F}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{FB5113DB-7A77-4994-B7F3-4AEA239B3CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C90B4C99-CABC-497B-AFCC-3414944A4391}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3735" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generate Tables" sheetId="1" r:id="rId1"/>
@@ -604,7 +604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5850,6 +5852,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q79" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5859,7 +5862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF23F58-F5E6-43E8-AD91-23A40ED8C925}">
   <dimension ref="A1:Q79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>